<commit_message>
Updates on BLDC controller
- added possbility to switch the Control mode while motor is spinning
- added support for Cruise control: activated by b_cruiseCtrlEna, where the target to set is n_cruiseMotTgt. (Needs small aditional handling on the application firmware to set the n_cruiseMotTgt properly to the current operation speed, immediately after activation via b_cruiseCtrlEna).
- extended Phase current measurements z_selPhaCurMeasABC : {iA,iB} = 0; {iB,iC} = 1; {iA,iC} = 2
- added interface for external motor angle measurement from as sensor, e.g., encoder. The selection can be done via b_angleMeasEna.
</commit_message>
<xml_diff>
--- a/03_CreateParamTable/tableParamType.xlsx
+++ b/03_CreateParamTable/tableParamType.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hoverboard-firmware-hack-FOC\01_Matlab\03_CreateParamTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bldc-motor-control-FOC\03_CreateParamTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="0" windowWidth="17280" windowHeight="8640" activeTab="1"/>
+    <workbookView xWindow="33030" yWindow="0" windowWidth="17280" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="95">
   <si>
     <t>Parameter</t>
   </si>
@@ -118,9 +118,6 @@
     <t>t_errQual</t>
   </si>
   <si>
-    <t>b_selPhaABCurrMeas</t>
-  </si>
-  <si>
     <t>cf_currFilt</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>Field weakening enable flag</t>
   </si>
   <si>
-    <t>Measured phase currents selection: {iA,iB} = 1 (default); {iB,iC} = 0</t>
-  </si>
-  <si>
     <t>Current filter coefficient</t>
   </si>
   <si>
@@ -262,31 +256,61 @@
     <t>cf_nKiLimProt</t>
   </si>
   <si>
+    <t>r_fieldWeakHi</t>
+  </si>
+  <si>
+    <t>r_fieldWeakLo</t>
+  </si>
+  <si>
+    <t>Maximum phase advance angle (only for SIN control type)</t>
+  </si>
+  <si>
+    <t>Back calculation gain for integral anti-windup (VLT_MODE and TRQ_MODE)</t>
+  </si>
+  <si>
+    <t>Current limit protection I gain (only for VLT_MODE and SPD_MODE)</t>
+  </si>
+  <si>
+    <t>Speed limit protection I gain (only for VLT_MODE and TRQ_MODE)</t>
+  </si>
+  <si>
+    <t>Input target High threshold for reaching maximum Field Weakening</t>
+  </si>
+  <si>
+    <t>Input target Low threshold for starting Field Weakening</t>
+  </si>
+  <si>
+    <t>b_angleMeasEna</t>
+  </si>
+  <si>
+    <t>b_cruiseCtrlEna</t>
+  </si>
+  <si>
     <t>id_fieldWeakMax</t>
   </si>
   <si>
-    <t>r_fieldWeakHi</t>
-  </si>
-  <si>
-    <t>r_fieldWeakLo</t>
-  </si>
-  <si>
-    <t>Maximum phase advance angle (only for SIN control type)</t>
-  </si>
-  <si>
-    <t>Back calculation gain for integral anti-windup (VLT_MODE and TRQ_MODE)</t>
-  </si>
-  <si>
-    <t>Current limit protection I gain (only for VLT_MODE and SPD_MODE)</t>
-  </si>
-  <si>
-    <t>Speed limit protection I gain (only for VLT_MODE and TRQ_MODE)</t>
-  </si>
-  <si>
-    <t>Input target High threshold for reaching maximum Field Weakening</t>
-  </si>
-  <si>
-    <t>Input target Low threshold for starting Field Weakening</t>
+    <t>n_cruiseMotTgt</t>
+  </si>
+  <si>
+    <t>n_polePairs</t>
+  </si>
+  <si>
+    <t>z_selPhaCurMeasABC</t>
+  </si>
+  <si>
+    <t>Enable flag for external mechanical motor angle sensor</t>
+  </si>
+  <si>
+    <t>Cruise control enable flag</t>
+  </si>
+  <si>
+    <t>Cruise control motor speed target</t>
+  </si>
+  <si>
+    <t>Number of motor pole pairs</t>
+  </si>
+  <si>
+    <t>Measured current phases selection: {iA,iB} = 0; {iB,iC} = 1; {iA,iC} = 2</t>
   </si>
 </sst>
 </file>
@@ -382,8 +406,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:D40" totalsRowShown="0">
-  <autoFilter ref="B3:D40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:D44" totalsRowShown="0">
+  <autoFilter ref="B3:D44"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Parameter"/>
     <tableColumn id="2" name="DataType"/>
@@ -656,15 +680,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -702,7 +726,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -710,7 +734,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -718,7 +742,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -726,7 +750,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -734,23 +758,23 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -758,23 +782,23 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -782,23 +806,23 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -806,55 +830,55 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -862,7 +886,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -870,7 +894,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -878,7 +902,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -886,15 +910,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -902,7 +926,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
@@ -910,7 +934,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -918,15 +942,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
         <v>24</v>
@@ -934,42 +958,74 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
-        <v>35</v>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -979,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D40"/>
+  <dimension ref="B3:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,7 +1058,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1013,7 +1069,7 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -1024,7 +1080,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -1035,381 +1091,425 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
         <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
         <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>52</v>
+      <c r="D31" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
         <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
         <v>24</v>
       </c>
-      <c r="D33" t="s">
-        <v>54</v>
+      <c r="D33" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>85</v>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>86</v>
+      <c r="D35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" t="s">
-        <v>56</v>
+      <c r="B37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" t="s">
-        <v>57</v>
+        <v>24</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C40" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" t="s">
-        <v>58</v>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>